<commit_message>
Complete Searching and sorting algorithms
</commit_message>
<xml_diff>
--- a/Semaster 1/Introduction to Computer Science with Contemporary Language/Assignments/Newton Raphson Method/newton_raphson_method.xlsx
+++ b/Semaster 1/Introduction to Computer Science with Contemporary Language/Assignments/Newton Raphson Method/newton_raphson_method.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RAO\Documents\GitHub\UBIT-Work\Semaster 1\Introduction to Computer Science with Contemporary Language\Assignments\Newton Raphson Method\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEED3B6-D578-49E5-9C73-C5EEC96408F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F535EEF-4D80-450C-986F-5745279D07AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{908026CA-B4F4-498F-BC8F-369ED82AEBE6}"/>
   </bookViews>
@@ -51,10 +51,10 @@
     <t>acceptance</t>
   </si>
   <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>y_dev</t>
+    <t>f(Xn)</t>
+  </si>
+  <si>
+    <t>f'(Xn)</t>
   </si>
 </sst>
 </file>
@@ -62,9 +62,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="173" formatCode="0.00000E+00"/>
-    <numFmt numFmtId="187" formatCode="0.0000000000000000000"/>
-    <numFmt numFmtId="195" formatCode="0.000000000000000000000000000"/>
+    <numFmt numFmtId="164" formatCode="0.00000E+00"/>
+    <numFmt numFmtId="165" formatCode="0.0000000000000000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000000000000000000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -103,9 +103,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="195" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,7 +423,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,7 +527,7 @@
         <v>-0.66666666666666674</v>
       </c>
       <c r="H9" t="str">
-        <f t="shared" ref="H8:H14" si="0">IF(ABS(E9)&gt;$B$4, "Not Accepted", "Accepted")</f>
+        <f t="shared" ref="H9:H12" si="0">IF(ABS(E9)&gt;$B$4, "Not Accepted", "Accepted")</f>
         <v>Not Accepted</v>
       </c>
     </row>
@@ -540,7 +540,7 @@
         <v>-0.66666666666666674</v>
       </c>
       <c r="E10">
-        <f t="shared" ref="E10:E14" si="2">D10^2 -D10-1</f>
+        <f t="shared" ref="E10:E12" si="2">D10^2 -D10-1</f>
         <v>0.11111111111111116</v>
       </c>
       <c r="F10">
@@ -586,7 +586,7 @@
         <v>5</v>
       </c>
       <c r="D12" s="4">
-        <f t="shared" ref="D12:D14" si="5">G11</f>
+        <f t="shared" ref="D12" si="5">G11</f>
         <v>-0.61803444782168193</v>
       </c>
       <c r="E12" s="3">
@@ -594,11 +594,11 @@
         <v>1.0265159331446227E-6</v>
       </c>
       <c r="F12">
-        <f t="shared" ref="F12:F14" si="6" xml:space="preserve"> 2*D12-1</f>
+        <f t="shared" ref="F12" si="6" xml:space="preserve"> 2*D12-1</f>
         <v>-2.2360688956433639</v>
       </c>
       <c r="G12">
-        <f t="shared" ref="G12:G14" si="7">D12-(E12/F12)</f>
+        <f t="shared" ref="G12" si="7">D12-(E12/F12)</f>
         <v>-0.61803398874998916</v>
       </c>
       <c r="H12" t="str">

</xml_diff>